<commit_message>
Small improvements to thesis
</commit_message>
<xml_diff>
--- a/thesis/Result_Matrix.xlsx
+++ b/thesis/Result_Matrix.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
   <si>
     <t>client-server</t>
   </si>
@@ -82,6 +82,24 @@
   </si>
   <si>
     <t>Audio and video stream handling included</t>
+  </si>
+  <si>
+    <t>Communicate verbally</t>
+  </si>
+  <si>
+    <t>Point to objects</t>
+  </si>
+  <si>
+    <t>Independent of operating system and hardware platforms</t>
+  </si>
+  <si>
+    <t>Multiple audio and video codecs integrated</t>
+  </si>
+  <si>
+    <t>Integrated support for gestures</t>
+  </si>
+  <si>
+    <t>Pause video feed</t>
   </si>
 </sst>
 </file>
@@ -2108,7 +2126,7 @@
   <dimension ref="B1:I43"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="B16" sqref="B16"/>
+      <selection activeCell="B25" sqref="B25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2277,8 +2295,36 @@
         <v>21</v>
       </c>
     </row>
-    <row r="22" spans="7:7" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B19" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B20" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="21" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B21" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" ht="15" x14ac:dyDescent="0.25">
+      <c r="B22" s="1" t="s">
+        <v>25</v>
+      </c>
       <c r="G22"/>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B23" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.2">
+      <c r="B24" s="1" t="s">
+        <v>27</v>
+      </c>
     </row>
     <row r="43" spans="9:9" ht="15" x14ac:dyDescent="0.25">
       <c r="I43"/>

</xml_diff>